<commit_message>
Tests with amputating legs
</commit_message>
<xml_diff>
--- a/python_helpers/modules_prost.xlsx
+++ b/python_helpers/modules_prost.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picch\Zomboid\mods\The-Only-Cure-But-Better\python_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715CBB47-AE5E-413C-A92F-864373F99F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079102F5-3F2E-4CF7-A83E-48DA20523F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Forearm" sheetId="1" r:id="rId1"/>
-    <sheet name="Hand" sheetId="8" r:id="rId2"/>
+    <sheet name="Models to make" sheetId="9" r:id="rId2"/>
+    <sheet name="Hand" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Forearm!$A$21:$C$45</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Hand!$G$1:$H$9</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Forearm!$A$21:$A$33</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">Hand!$G$1:$H$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,23 +59,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
   <si>
     <t>Base</t>
   </si>
   <si>
-    <t>Strap</t>
-  </si>
-  <si>
     <t>Top</t>
   </si>
   <si>
-    <t>Leather Strap</t>
-  </si>
-  <si>
-    <t>Sheet Strap</t>
-  </si>
-  <si>
     <t>Leather Base</t>
   </si>
   <si>
@@ -121,6 +113,15 @@
   </si>
   <si>
     <t>Attack</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Prosthesis Base</t>
   </si>
 </sst>
 </file>
@@ -191,12 +192,15 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{089432D4-765F-4D64-B008-B197BCD45818}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+  <queryTableRefresh nextId="4" unboundColumnsRight="1">
+    <queryTableFields count="2">
       <queryTableField id="1" name="Strap" tableColumnId="1"/>
-      <queryTableField id="2" name="Custom1.Base" tableColumnId="2"/>
-      <queryTableField id="3" name="Custom2.Top" tableColumnId="3"/>
+      <queryTableField id="2" dataBound="0" tableColumnId="2"/>
     </queryTableFields>
+    <queryTableDeletedFields count="2">
+      <deletedField name="Custom1.Base"/>
+      <deletedField name="Custom2.Top"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
@@ -213,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B07FBF0-362F-422A-B533-B04733538332}" name="Tabella3" displayName="Tabella3" ref="E1:G4" totalsRowShown="0">
-  <autoFilter ref="E1:G4" xr:uid="{1B07FBF0-362F-422A-B533-B04733538332}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B07FBF0-362F-422A-B533-B04733538332}" name="Tabella3" displayName="Tabella3" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{1B07FBF0-362F-422A-B533-B04733538332}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{259F1B0E-4EB9-43B5-8366-52635591EA1F}" name="Base"/>
     <tableColumn id="2" xr3:uid="{0933CE51-FD2A-4EFD-8A9B-60A63369D05F}" name="Speed Mod"/>
@@ -225,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F9CD85DA-1148-4516-AE05-483E13AA8A27}" name="Tabella4" displayName="Tabella4" ref="I1:L5" totalsRowShown="0">
-  <autoFilter ref="I1:L5" xr:uid="{F9CD85DA-1148-4516-AE05-483E13AA8A27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F9CD85DA-1148-4516-AE05-483E13AA8A27}" name="Tabella4" displayName="Tabella4" ref="E1:H5" totalsRowShown="0">
+  <autoFilter ref="E1:H5" xr:uid="{F9CD85DA-1148-4516-AE05-483E13AA8A27}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F9C40781-51DD-49F2-AF22-6520AAC118CF}" name="Top"/>
     <tableColumn id="2" xr3:uid="{7EB66B28-6105-4793-9EBD-58D473423AF3}" name="Durability"/>
@@ -238,30 +242,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65991F0A-756B-41E7-ADFE-3DCB5C0934D7}" name="Tabella2" displayName="Tabella2" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{65991F0A-756B-41E7-ADFE-3DCB5C0934D7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7C21E179-C017-43A9-86E0-FFD0F0FC828A}" name="Strap"/>
-    <tableColumn id="2" xr3:uid="{C2023241-6999-4A03-8689-3206D52881E1}" name="Speed Mod"/>
-    <tableColumn id="3" xr3:uid="{D043B9D8-D184-42B6-975E-667503E5724B}" name="Durability"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F948790C-FA2D-4239-82A4-8D93A4BE7A6B}" name="Forearm_Modules" displayName="Forearm_Modules" ref="A21:C45" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A21:C45" xr:uid="{F948790C-FA2D-4239-82A4-8D93A4BE7A6B}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{768D63FA-ABD5-439F-B9F6-8B5D3FE1AB58}" uniqueName="1" name="Strap" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A2956E84-4689-4108-87ED-D817361ED8F0}" uniqueName="2" name="Base" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{3458008C-F1DE-4ECA-9349-E55AC6DEF23F}" uniqueName="3" name="Forearm" queryTableFieldId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F948790C-FA2D-4239-82A4-8D93A4BE7A6B}" name="Forearm_Modules" displayName="Forearm_Modules" ref="A21:B33" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A21:B33" xr:uid="{F948790C-FA2D-4239-82A4-8D93A4BE7A6B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{768D63FA-ABD5-439F-B9F6-8B5D3FE1AB58}" uniqueName="1" name="Base" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A2956E84-4689-4108-87ED-D817361ED8F0}" uniqueName="2" name="Forearm" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{87ED2382-E460-4FF6-8575-4D2FE4E1A118}" name="Tabella310" displayName="Tabella310" ref="A1:C3" totalsRowShown="0">
   <autoFilter ref="A1:C3" xr:uid="{87ED2382-E460-4FF6-8575-4D2FE4E1A118}"/>
   <tableColumns count="3">
@@ -273,7 +264,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F18EB07D-97E6-42D4-B2D8-5D796CB3EB61}" name="Tabella411" displayName="Tabella411" ref="A5:C9" totalsRowShown="0">
   <autoFilter ref="A5:C9" xr:uid="{F18EB07D-97E6-42D4-B2D8-5D796CB3EB61}"/>
   <tableColumns count="3">
@@ -285,7 +276,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9EE49BF-4899-4F1E-8CE1-694AC5CB2209}" name="Hand_modules" displayName="Hand_modules" ref="G1:H9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="G1:H9" xr:uid="{A9EE49BF-4899-4F1E-8CE1-694AC5CB2209}"/>
   <tableColumns count="2">
@@ -594,89 +585,71 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6903C0B-FFA6-4A1C-8589-50764749E446}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A7" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
     <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -688,364 +661,254 @@
         <v>6</v>
       </c>
       <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>4</v>
+      </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I5" t="s">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <f>ROWS(Forearm_Modules[])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <f>F9*2</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22">
-        <f>ROWS(Forearm_Modules[])</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23">
-        <f>F22*2</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>3</v>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>4</v>
       </c>
       <c r="B27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>4</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>3</v>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD56C17-BE24-4D02-A517-6544AB9A874B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CA4D0A-0B1E-4D6D-B693-37F1F321F792}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -1067,30 +930,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <f>ROWS(Hand_modules[])</f>
@@ -1099,16 +962,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K3">
         <f>K2*2</f>
@@ -1117,71 +980,71 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
         <v>7</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forgot to reneable stuff and more things in preparation for modular prost
</commit_message>
<xml_diff>
--- a/python_helpers/modules_prost.xlsx
+++ b/python_helpers/modules_prost.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picch\Zomboid\mods\The-Only-Cure-But-Better\python_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079102F5-3F2E-4CF7-A83E-48DA20523F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB0F745-B3F7-410A-94FD-48CD902FC819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
+    <workbookView xWindow="-28690" yWindow="-30" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Forearm" sheetId="1" r:id="rId1"/>
-    <sheet name="Models to make" sheetId="9" r:id="rId2"/>
-    <sheet name="Hand" sheetId="8" r:id="rId3"/>
+    <sheet name="StuffToImport" sheetId="10" r:id="rId2"/>
+    <sheet name="Models to make" sheetId="9" r:id="rId3"/>
+    <sheet name="Hand" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Forearm!$A$21:$A$33</definedName>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">Hand!$G$1:$H$9</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Hand!$G$1:$H$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
   <si>
     <t>Base</t>
   </si>
@@ -122,6 +123,33 @@
   </si>
   <si>
     <t>Prosthesis Base</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>WoodenBase</t>
+  </si>
+  <si>
+    <t>MetalBase</t>
+  </si>
+  <si>
+    <t>LeatherBase</t>
+  </si>
+  <si>
+    <t>WoodenHook</t>
+  </si>
+  <si>
+    <t>MetalHook</t>
+  </si>
+  <si>
+    <t>MetalHand</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>LeatherBase_MetalHand</t>
   </si>
 </sst>
 </file>
@@ -253,6 +281,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}" name="BaseTable" displayName="BaseTable" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{431049C1-BE90-4307-881E-9C7DF8E03E88}" name="Base"/>
+    <tableColumn id="2" xr3:uid="{EDA28F2C-75D2-4712-9624-6BC385A54AEE}" name="Durability"/>
+    <tableColumn id="3" xr3:uid="{E41D3B99-F5C2-4367-A8E5-5DBCEBF9E744}" name="Speed"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}" name="TopTable" displayName="TopTable" ref="E1:G4" totalsRowShown="0">
+  <autoFilter ref="E1:G4" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1EBB0807-5D0D-4CE0-932E-F266B699B167}" name="Top"/>
+    <tableColumn id="2" xr3:uid="{322E0465-3850-435C-A129-C934CA1F55D7}" name="Durability"/>
+    <tableColumn id="3" xr3:uid="{7FBD2018-B0C0-4D3E-8B56-4AB5D27DB310}" name="Speed"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{87ED2382-E460-4FF6-8575-4D2FE4E1A118}" name="Tabella310" displayName="Tabella310" ref="A1:C3" totalsRowShown="0">
   <autoFilter ref="A1:C3" xr:uid="{87ED2382-E460-4FF6-8575-4D2FE4E1A118}"/>
   <tableColumns count="3">
@@ -264,7 +316,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F18EB07D-97E6-42D4-B2D8-5D796CB3EB61}" name="Tabella411" displayName="Tabella411" ref="A5:C9" totalsRowShown="0">
   <autoFilter ref="A5:C9" xr:uid="{F18EB07D-97E6-42D4-B2D8-5D796CB3EB61}"/>
   <tableColumns count="3">
@@ -276,7 +328,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9EE49BF-4899-4F1E-8CE1-694AC5CB2209}" name="Hand_modules" displayName="Hand_modules" ref="G1:H9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="G1:H9" xr:uid="{A9EE49BF-4899-4F1E-8CE1-694AC5CB2209}"/>
   <tableColumns count="2">
@@ -878,16 +930,133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F82667-3ED3-4C29-BED2-BFFA7CD365A6}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD56C17-BE24-4D02-A517-6544AB9A874B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -908,7 +1077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CA4D0A-0B1E-4D6D-B693-37F1F321F792}">
   <dimension ref="A1:K9"/>
   <sheetViews>

</xml_diff>

<commit_message>
automatically generating item via script
</commit_message>
<xml_diff>
--- a/python_helpers/modules_prost.xlsx
+++ b/python_helpers/modules_prost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picch\Zomboid\mods\The-Only-Cure-But-Better\python_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB0F745-B3F7-410A-94FD-48CD902FC819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387915E-70D4-4E3F-915B-D6AE6F7A0AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28690" yWindow="-30" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Forearm" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
   <si>
     <t>Base</t>
   </si>
@@ -146,10 +146,22 @@
     <t>MetalHand</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>LeatherBase_MetalHand</t>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Display Name</t>
   </si>
 </sst>
 </file>
@@ -281,24 +293,28 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}" name="BaseTable" displayName="BaseTable" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}" name="BaseTable" displayName="BaseTable" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{431049C1-BE90-4307-881E-9C7DF8E03E88}" name="Base"/>
-    <tableColumn id="2" xr3:uid="{EDA28F2C-75D2-4712-9624-6BC385A54AEE}" name="Durability"/>
-    <tableColumn id="3" xr3:uid="{E41D3B99-F5C2-4367-A8E5-5DBCEBF9E744}" name="Speed"/>
+    <tableColumn id="2" xr3:uid="{EDA28F2C-75D2-4712-9624-6BC385A54AEE}" name="Display Name"/>
+    <tableColumn id="3" xr3:uid="{E41D3B99-F5C2-4367-A8E5-5DBCEBF9E744}" name="Durability"/>
+    <tableColumn id="4" xr3:uid="{A4A34E27-118C-400A-94AE-EE479746791A}" name="Speed"/>
+    <tableColumn id="5" xr3:uid="{D8EE11BC-C89B-4EB8-B2E7-F932A6650D93}" name="Weight"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}" name="TopTable" displayName="TopTable" ref="E1:G4" totalsRowShown="0">
-  <autoFilter ref="E1:G4" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}" name="TopTable" displayName="TopTable" ref="I1:M4" totalsRowShown="0">
+  <autoFilter ref="I1:M4" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1EBB0807-5D0D-4CE0-932E-F266B699B167}" name="Top"/>
-    <tableColumn id="2" xr3:uid="{322E0465-3850-435C-A129-C934CA1F55D7}" name="Durability"/>
-    <tableColumn id="3" xr3:uid="{7FBD2018-B0C0-4D3E-8B56-4AB5D27DB310}" name="Speed"/>
+    <tableColumn id="2" xr3:uid="{322E0465-3850-435C-A129-C934CA1F55D7}" name="Display Name"/>
+    <tableColumn id="3" xr3:uid="{7FBD2018-B0C0-4D3E-8B56-4AB5D27DB310}" name="Durability"/>
+    <tableColumn id="4" xr3:uid="{51C1ACCA-DC4A-440E-8199-A861E3E24917}" name="Speed"/>
+    <tableColumn id="5" xr3:uid="{BABFB9E4-608C-4C95-85EC-A92D102D3C99}" name="Weight"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -931,108 +947,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F82667-3ED3-4C29-BED2-BFFA7CD365A6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" customWidth="1"/>
     <col min="6" max="6" width="9.54296875" customWidth="1"/>
     <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="F2">
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="L2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>75</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="F3">
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="L3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="F4">
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4">
         <v>15</v>
       </c>
-      <c r="G4">
+      <c r="L4">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="M4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generating normal item for assembly
</commit_message>
<xml_diff>
--- a/python_helpers/modules_prost.xlsx
+++ b/python_helpers/modules_prost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picch\Zomboid\mods\The-Only-Cure-But-Better\python_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387915E-70D4-4E3F-915B-D6AE6F7A0AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C88644C-3D08-403F-997C-72D39244D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CDD28935-60E2-42C1-AE58-DBE5C0F6C0C4}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Base</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Display Name</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Tooltip</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -293,28 +302,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}" name="BaseTable" displayName="BaseTable" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}" name="BaseTable" displayName="BaseTable" ref="A1:G4" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{4F961ED7-02EB-485E-BB34-6E6AAD4ED2F5}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{431049C1-BE90-4307-881E-9C7DF8E03E88}" name="Base"/>
     <tableColumn id="2" xr3:uid="{EDA28F2C-75D2-4712-9624-6BC385A54AEE}" name="Display Name"/>
     <tableColumn id="3" xr3:uid="{E41D3B99-F5C2-4367-A8E5-5DBCEBF9E744}" name="Durability"/>
     <tableColumn id="4" xr3:uid="{A4A34E27-118C-400A-94AE-EE479746791A}" name="Speed"/>
     <tableColumn id="5" xr3:uid="{D8EE11BC-C89B-4EB8-B2E7-F932A6650D93}" name="Weight"/>
+    <tableColumn id="6" xr3:uid="{CCEC0405-6B00-4E62-8682-7B8866A93EAF}" name="Icon"/>
+    <tableColumn id="7" xr3:uid="{C41242F3-B269-4FFA-B28D-3094AD3A80E5}" name="Tooltip"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}" name="TopTable" displayName="TopTable" ref="I1:M4" totalsRowShown="0">
-  <autoFilter ref="I1:M4" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}" name="TopTable" displayName="TopTable" ref="A13:G16" totalsRowShown="0">
+  <autoFilter ref="A13:G16" xr:uid="{FA3D76C9-DFD5-4F3B-A1AC-D4D2880E983B}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1EBB0807-5D0D-4CE0-932E-F266B699B167}" name="Top"/>
     <tableColumn id="2" xr3:uid="{322E0465-3850-435C-A129-C934CA1F55D7}" name="Display Name"/>
     <tableColumn id="3" xr3:uid="{7FBD2018-B0C0-4D3E-8B56-4AB5D27DB310}" name="Durability"/>
     <tableColumn id="4" xr3:uid="{51C1ACCA-DC4A-440E-8199-A861E3E24917}" name="Speed"/>
     <tableColumn id="5" xr3:uid="{BABFB9E4-608C-4C95-85EC-A92D102D3C99}" name="Weight"/>
+    <tableColumn id="6" xr3:uid="{431BD633-5734-4F7E-AC5C-A5C3E6B55DC7}" name="Icon"/>
+    <tableColumn id="7" xr3:uid="{D7544ABF-F817-4256-A65B-527660E471B4}" name="Tooltip"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -947,10 +960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F82667-3ED3-4C29-BED2-BFFA7CD365A6}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,7 +980,7 @@
     <col min="13" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,23 +996,14 @@
       <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1015,23 +1019,11 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1047,23 +1039,8 @@
       <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>7</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1079,23 +1056,83 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="K4">
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="L4">
+      <c r="D16">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>